<commit_message>
feat: - dateformat Attribute - NumberFormat Attribute
</commit_message>
<xml_diff>
--- a/example/writer.xlsx
+++ b/example/writer.xlsx
@@ -15,105 +15,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>序号</t>
   </si>
   <si>
+    <t>名称</t>
+  </si>
+  <si>
     <t>密码</t>
   </si>
   <si>
-    <t>名称</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7258	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">羴趣瞅傷	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mUTGXC	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7376	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">嚺逨返娨	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CT1hKT	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3959	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">恒硉灸垻	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2qtxrd	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7689	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">峄鱽渄灒	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LBcp8T	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1091	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">莳弄鄢鵊	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hodnl7	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4351	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">姤玥厃絾	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SZE78t	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0096	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">捥閾耏愎	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0Eql4U	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1571	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">濠龰陑電	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLVVYk	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3200	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">肭殹鍟膄	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dS5SuY	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4437	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">帓艘卵鷜	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9p6qSY	</t>
+    <t>登录时间</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4286	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">糤蕅湔綞	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V8DB3a	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-08-05 01:35:01	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1318	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">慈捦鶏锃	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qgmw53	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8402	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">舲亅犙晘	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOXOOC	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0402	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">罇縍畁煆	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LxQbKC	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5998	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">繿輂氳枾	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5wI1yM	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3665	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">挒勾诗瑇	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL0M5z	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7628	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">葁盺悗嵕	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4ixc7l	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3207	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">婟侐都雖	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T9Xquu	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8596	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">擌寸牣犬	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uUPx3P	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2300	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">臽裯犈荐	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5EMXT1	</t>
   </si>
 </sst>
 </file>
@@ -141,19 +147,15 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,7 +455,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +463,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,115 +473,148 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: - 完善xlsxwriter Handler
</commit_message>
<xml_diff>
--- a/example/writer.xlsx
+++ b/example/writer.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="1111" sheetId="1" r:id="rId4"/>
+    <sheet name="1111" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>序号</t>
   </si>
@@ -29,113 +28,110 @@
     <t>登录时间</t>
   </si>
   <si>
-    <t xml:space="preserve">4286	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">糤蕅湔綞	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V8DB3a	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-05 01:35:01	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1318	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">慈捦鶏锃	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qgmw53	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8402	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">舲亅犙晘	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOXOOC	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0402	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">罇縍畁煆	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LxQbKC	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5998	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">繿輂氳枾	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5wI1yM	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3665	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">挒勾诗瑇	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NL0M5z	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7628	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">葁盺悗嵕	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4ixc7l	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3207	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">婟侐都雖	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T9Xquu	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8596	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">擌寸牣犬	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uUPx3P	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2300	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">臽裯犈荐	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5EMXT1	</t>
+    <t xml:space="preserve">5229	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">哾喂溠痚	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2jGEhq	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-08-05 13:17:25	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4430	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">踍縮膁思	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z9hp8v	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6950	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">冤牲华簝	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K0mOSj	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0262	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">槴嶿箕滋	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tXn9qA	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0362	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">姳懞昂僰	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YWNZ17	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6349	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">璿薶寶脔	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le7bmu	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7490	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鶿漅骚倠	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rVKHFW	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9204	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鯣鼷谭拼	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q5encx	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8061	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">塇鼄芋璆	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aUUI8S	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3282	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">翲縬蒫湚	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6hp8Pq	</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,21 +143,25 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -240,7 +240,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -275,7 +274,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -451,17 +449,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -618,17 +611,6 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>